<commit_message>
budget additions and added qPCR result merged
</commit_message>
<xml_diff>
--- a/MigratoryStationary/Documents/MigratoryHB_Budget.xlsx
+++ b/MigratoryStationary/Documents/MigratoryHB_Budget.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28125"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="880" yWindow="10140" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
   <si>
     <t>Beekeeper</t>
   </si>
@@ -152,6 +152,12 @@
   </si>
   <si>
     <t>ZAC is owed:</t>
+  </si>
+  <si>
+    <t>pipettes, freezer boxes, liquid nitrogen</t>
+  </si>
+  <si>
+    <t>ACTUAL FUNDS RECEIVED=</t>
   </si>
 </sst>
 </file>
@@ -268,7 +274,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -280,8 +286,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -294,18 +302,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -573,7 +584,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -581,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -762,8 +773,8 @@
         <v>420</v>
       </c>
       <c r="F11">
-        <f>212.77+177.12+24.61+198.03</f>
-        <v>612.53</v>
+        <f>212.77+177.12+24.61+198.03+15.8</f>
+        <v>628.32999999999993</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -798,7 +809,7 @@
       </c>
       <c r="F13">
         <f>SUM(F8:F12)</f>
-        <v>1099.4100000000001</v>
+        <v>1115.21</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -833,7 +844,7 @@
         <v>640</v>
       </c>
       <c r="F16">
-        <v>666</v>
+        <v>668.34</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -966,82 +977,106 @@
     <row r="25" spans="1:12">
       <c r="A25" s="5"/>
       <c r="B25" s="2" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25">
-        <v>5.08</v>
+        <v>50.53</v>
       </c>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="5"/>
       <c r="B26" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26">
-        <v>73.400000000000006</v>
+        <v>5.08</v>
       </c>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="5"/>
       <c r="B27" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
-      <c r="F27" s="9">
-        <v>420.66</v>
-      </c>
-      <c r="K27">
-        <v>180</v>
-      </c>
-      <c r="L27">
-        <f>K27*3</f>
-        <v>540</v>
+      <c r="F27">
+        <v>73.400000000000006</v>
       </c>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="5"/>
-      <c r="B28" s="2"/>
+      <c r="B28" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="C28" s="3"/>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="9">
+        <v>420.66</v>
+      </c>
+      <c r="K28">
+        <v>180</v>
+      </c>
+      <c r="L28">
+        <f>K28*3</f>
+        <v>540</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="5"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E29" s="6">
         <f>SUM(E16:E23)</f>
         <v>3006</v>
       </c>
-      <c r="F28">
+      <c r="F29">
         <f>SUM(F16:F23)</f>
-        <v>831</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="F29">
-        <f>SUM(F5+F13+F28)</f>
-        <v>3930.41</v>
-      </c>
-      <c r="G29">
-        <f>F30-F29</f>
-        <v>1538.9899999999998</v>
+        <v>833.34</v>
       </c>
     </row>
     <row r="30" spans="1:12">
-      <c r="D30" s="7" t="s">
+      <c r="F30">
+        <f>SUM(F5+F13+F29)</f>
+        <v>3948.55</v>
+      </c>
+      <c r="G30">
+        <f>F32-F30</f>
+        <v>1520.8499999999995</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="D31" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E30" s="7">
-        <f>SUM(E5,E13,E28)</f>
+      <c r="E31" s="7">
+        <f>SUM(E5,E13,E29)</f>
         <v>5875</v>
       </c>
-      <c r="F30">
+    </row>
+    <row r="32" spans="1:12">
+      <c r="D32" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10">
         <v>5469.4</v>
+      </c>
+    </row>
+    <row r="33" spans="7:7">
+      <c r="G33">
+        <f>G30-420.66</f>
+        <v>1100.1899999999994</v>
       </c>
     </row>
   </sheetData>
@@ -1057,10 +1092,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1150,6 +1185,26 @@
         <v>561.54</v>
       </c>
     </row>
+    <row r="6" spans="1:6">
+      <c r="B6">
+        <f>SUM(B2:B4)</f>
+        <v>206.07999999999998</v>
+      </c>
+      <c r="C6">
+        <f>SUM(C2:C4)</f>
+        <v>587.91999999999996</v>
+      </c>
+      <c r="D6">
+        <f>SUM(D2:D3)</f>
+        <v>40.409999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="D7">
+        <f>C6+D6</f>
+        <v>628.32999999999993</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>